<commit_message>
feat: add GraphAlq component for displaying rental metrics and charts
- Created a new Vue component `GraphAlq.vue` to visualize total rentals and inventory value.
- Integrated `vue-echarts` for rendering charts with options for line, bar, and pie charts.
- Implemented loading states and error handling for data fetching from ReportService and RentalService.
- Added a PostCSS configuration file for styling.
</commit_message>
<xml_diff>
--- a/_docs/trim_02/Contextualizacion Proyecto/Porcentaje de codificacion total.xlsx
+++ b/_docs/trim_02/Contextualizacion Proyecto/Porcentaje de codificacion total.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\AXXION_SYSTEM_\_docs\trim_02\Contextualizacion Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5E961F-F5C8-480B-B833-373A2D22F0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49793A34-4E1D-4777-9417-5286377835EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD96AF1-C494-414E-A4C6-796DD518F531}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="65">
   <si>
     <t>RF</t>
   </si>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE07042-B933-4627-BAC2-B36C8B2EB8A1}">
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,11 +874,11 @@
       </c>
       <c r="G5" s="17">
         <f>I5/I4</f>
-        <v>0.78735632183908044</v>
+        <v>0.79885057471264365</v>
       </c>
       <c r="I5" s="15">
         <f>COUNTIF(C2:E59,"x")</f>
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J5" s="16" t="s">
         <v>64</v>
@@ -1604,8 +1604,12 @@
       <c r="C50" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="14">

</xml_diff>